<commit_message>
grupos carga masiva docentes ok
</commit_message>
<xml_diff>
--- a/static/formatos/base.xlsx
+++ b/static/formatos/base.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sistemas\PycharmProjects\Andes\static\formatos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>ESTRATEGIA DE FORMACIÓN Y ACCESO PARA LA APROPIACIÓN PEDAGÓGICA DE LAS TIC</t>
   </si>
@@ -40,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -109,6 +115,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -126,12 +144,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -151,6 +163,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257177</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>39688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1809751</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>392641</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257177" y="39688"/>
+          <a:ext cx="1552574" cy="1638828"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -242,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +336,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -310,6 +388,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,67 +590,67 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="9" customWidth="1"/>
-    <col min="2" max="16" width="30" style="9" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="30.5703125" style="5" customWidth="1"/>
+    <col min="2" max="16" width="30" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="2:9" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="4" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="2:9" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="2:9" s="7" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="2:9" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:9" s="7" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" s="3" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:9" s="7" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -574,4 +669,96 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" style="5" customWidth="1"/>
+    <col min="2" max="16" width="30" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="7" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="2:9" s="7" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:9" s="7" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:9" s="7" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:XFD4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>